<commit_message>
make small minor changes
</commit_message>
<xml_diff>
--- a/tmpdir/file.xlsx
+++ b/tmpdir/file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="61">
   <si>
     <t>Banner ID</t>
   </si>
@@ -179,7 +179,34 @@
     <t>A00015222</t>
   </si>
   <si>
-    <t>A00015578</t>
+    <t>A00019098</t>
+  </si>
+  <si>
+    <t>the latest student</t>
+  </si>
+  <si>
+    <t>latest.student@aun.edu.ng</t>
+  </si>
+  <si>
+    <t>A00019099</t>
+  </si>
+  <si>
+    <t>latest.students@aun.edu.ng</t>
+  </si>
+  <si>
+    <t>the latest students</t>
+  </si>
+  <si>
+    <t>A00015518</t>
+  </si>
+  <si>
+    <t>A00015654</t>
+  </si>
+  <si>
+    <t>Some New Student</t>
+  </si>
+  <si>
+    <t>student@aun.edu.ng</t>
   </si>
 </sst>
 </file>
@@ -567,7 +594,7 @@
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="D2" sqref="D2"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,11 +728,11 @@
       <c r="S6" s="9">
         <v>42166</v>
       </c>
-      <c r="T6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>15</v>
+      <c r="T6" s="5">
+        <v>42333</v>
+      </c>
+      <c r="U6" s="5">
+        <v>42334</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>15</v>
@@ -796,6 +823,12 @@
       <c r="S7" t="s">
         <v>12</v>
       </c>
+      <c r="T7" t="s">
+        <v>11</v>
+      </c>
+      <c r="U7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -849,6 +882,12 @@
       <c r="S8" t="s">
         <v>11</v>
       </c>
+      <c r="T8" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -902,6 +941,12 @@
       <c r="S9" t="s">
         <v>11</v>
       </c>
+      <c r="T9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -952,6 +997,12 @@
       <c r="S10" t="s">
         <v>12</v>
       </c>
+      <c r="T10" t="s">
+        <v>11</v>
+      </c>
+      <c r="U10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
@@ -1007,6 +1058,12 @@
       <c r="S11" s="10" t="s">
         <v>9</v>
       </c>
+      <c r="T11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U11" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
@@ -1062,6 +1119,12 @@
       <c r="S12" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="T12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="U12" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
@@ -1115,6 +1178,12 @@
       <c r="S13" s="10" t="s">
         <v>9</v>
       </c>
+      <c r="T13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
@@ -1144,6 +1213,12 @@
       <c r="K14" s="10" t="s">
         <v>9</v>
       </c>
+      <c r="T14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="U14" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
@@ -1176,6 +1251,12 @@
       <c r="S15" t="s">
         <v>9</v>
       </c>
+      <c r="T15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="U15" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -1196,10 +1277,16 @@
       <c r="S16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>45</v>
@@ -1216,78 +1303,219 @@
       <c r="S17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S18" t="s">
+        <v>12</v>
+      </c>
+      <c r="T18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U19" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" t="s">
+        <v>9</v>
+      </c>
+      <c r="O20" t="s">
+        <v>11</v>
+      </c>
+      <c r="P20" t="s">
+        <v>12</v>
+      </c>
+      <c r="R20" t="s">
+        <v>11</v>
+      </c>
+      <c r="T20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>

</xml_diff>